<commit_message>
Updates to form handling.
</commit_message>
<xml_diff>
--- a/Arduino/SignalGenerator/SignalGenerator.xlsx
+++ b/Arduino/SignalGenerator/SignalGenerator.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaap\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="0" windowWidth="25290" windowHeight="11490"/>
+    <workbookView xWindow="2280" yWindow="0" windowWidth="20715" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>prescale</t>
   </si>
@@ -27,9 +32,6 @@
     <t>top</t>
   </si>
   <si>
-    <t>time unit</t>
-  </si>
-  <si>
     <t>frequency</t>
   </si>
   <si>
@@ -43,6 +45,24 @@
   </si>
   <si>
     <t>Clock frq.</t>
+  </si>
+  <si>
+    <t>ICR1 (H/L)</t>
+  </si>
+  <si>
+    <t>top start</t>
+  </si>
+  <si>
+    <t>top end</t>
+  </si>
+  <si>
+    <t>duty</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>top time</t>
   </si>
 </sst>
 </file>
@@ -78,8 +98,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -352,7 +378,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -360,38 +386,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:I14"/>
+  <dimension ref="C1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="10.140625" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>16000000</v>
       </c>
       <c r="D2">
         <v>65536</v>
       </c>
-    </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -399,19 +428,34 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1</v>
       </c>
@@ -434,8 +478,23 @@
         <f>1/H5</f>
         <v>244.140625</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>16</v>
+      </c>
+      <c r="L5">
+        <v>16</v>
+      </c>
+      <c r="M5">
+        <v>1000000</v>
+      </c>
+      <c r="O5">
+        <v>65536</v>
+      </c>
+      <c r="Q5">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>8</v>
       </c>
@@ -454,13 +513,25 @@
         <f>1/H7</f>
         <v>30.517578125</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>8163</v>
+      </c>
+      <c r="M7">
+        <v>244</v>
+      </c>
+      <c r="O7">
+        <v>65536</v>
+      </c>
+      <c r="Q7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>64</v>
       </c>
       <c r="D9">
-        <v>65536</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f>G7*64</f>
@@ -468,20 +539,43 @@
       </c>
       <c r="H9">
         <f>D9*G9</f>
-        <v>2.0971519999999999</v>
+        <v>3.1999999999999999E-5</v>
       </c>
       <c r="I9">
         <f>1/H9</f>
-        <v>0.476837158203125</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+        <v>31250</v>
+      </c>
+      <c r="K9">
+        <v>1041</v>
+      </c>
+      <c r="M9">
+        <v>30</v>
+      </c>
+      <c r="O9">
+        <v>31250</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F13" t="b">
         <f>(D2&lt;F14)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>50</v>
+      </c>
+      <c r="K13">
+        <f>1/J13</f>
+        <v>0.02</v>
+      </c>
+      <c r="L13">
+        <f>K13/G9</f>
+        <v>625</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>250</v>
       </c>
@@ -496,5 +590,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>